<commit_message>
corrected spells in spell sheet removed duplicates and UA spells
various corrections in other excel sheets, created initial files for 
testing

added armor roll in hoard roll

finished random spell script
</commit_message>
<xml_diff>
--- a/potions.xlsx
+++ b/potions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB43E696-D9E7-45F3-9615-DC9186440519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEC4257-F09B-4C82-B0A7-DA05FAE3E07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -675,9 +686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06607DA-061F-4581-816A-E1249043B1E8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -766,6 +777,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -857,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37985686-3E50-4889-AC5C-E298EE954F37}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>

</xml_diff>